<commit_message>
added contrain sketched to reflect FSAE rules
</commit_message>
<xml_diff>
--- a/Documents/Master Parts List.xlsx
+++ b/Documents/Master Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\Capstone\capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394AA6D5-6142-4720-AC26-C28929B5EF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE9C87-F17A-48F3-B8F0-97611103F91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7830" yWindow="80" windowWidth="13400" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>P/N</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Motor Bracket</t>
+  </si>
+  <si>
+    <t>cockpit opening template</t>
+  </si>
+  <si>
+    <t>cockpit internal cross-section</t>
   </si>
 </sst>
 </file>
@@ -205,19 +211,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,31 +523,29 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="5"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>230000</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>240000</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -847,6 +850,18 @@
       <c r="A47">
         <f>A46+1</f>
         <v>240003</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <f>A47+1</f>
+        <v>240004</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the rear suspension sketches
</commit_message>
<xml_diff>
--- a/Documents/Master Parts List.xlsx
+++ b/Documents/Master Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\Capstone\capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346EFB0B-D1A4-4C4A-8000-FA48DF2EAEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DABF86-71C7-4304-83A6-32B550307A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7830" yWindow="80" windowWidth="16560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>P/N</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>REV1 suspension assembly front passenger</t>
+  </si>
+  <si>
+    <t>REV1 suspension assembly rear driver</t>
+  </si>
+  <si>
+    <t>REV1 suspension assembly rear passenger</t>
   </si>
 </sst>
 </file>
@@ -509,15 +515,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -884,6 +890,24 @@
       </c>
       <c r="B50" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <f>A50+1</f>
+        <v>240007</v>
+      </c>
+      <c r="B51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <f>A51+1</f>
+        <v>240008</v>
+      </c>
+      <c r="B52" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more stuffs, sketches for REV1
</commit_message>
<xml_diff>
--- a/Documents/Master Parts List.xlsx
+++ b/Documents/Master Parts List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\Capstone\capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DABF86-71C7-4304-83A6-32B550307A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257E7869-9E1E-46A9-A947-67F1DD2CFDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7830" yWindow="80" windowWidth="16560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="7830" yWindow="80" windowWidth="16560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>P/N</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>REV1 suspension assembly rear passenger</t>
+  </si>
+  <si>
+    <t>REV1 steering rack assembly</t>
+  </si>
+  <si>
+    <t>REV1 pedal assembly</t>
   </si>
 </sst>
 </file>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -910,6 +916,24 @@
         <v>45</v>
       </c>
     </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <f>A52+1</f>
+        <v>240009</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <f>A53+1</f>
+        <v>240010</v>
+      </c>
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
front suspension arms and bracket sketches
</commit_message>
<xml_diff>
--- a/Documents/Master Parts List.xlsx
+++ b/Documents/Master Parts List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\University\Capstone\capstone\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C736873-B74C-41C2-B506-06D1EF1D2B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52627CD6-862C-49F3-BC68-D65113F0BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1530" yWindow="460" windowWidth="16560" windowHeight="13220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>P/N</t>
   </si>
@@ -243,12 +243,27 @@
   </si>
   <si>
     <t>Suspension Rod End Adapter</t>
+  </si>
+  <si>
+    <t>High-Load Ball Joint Rod End</t>
+  </si>
+  <si>
+    <t>McMaster</t>
+  </si>
+  <si>
+    <t>4482T6</t>
+  </si>
+  <si>
+    <t>Front Upper A-Arm, Assembly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,6 +328,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -978,7 +994,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
-        <f t="shared" ref="A42:A65" si="1">A41+1</f>
+        <f t="shared" ref="A42:A67" si="1">A41+1</f>
         <v>240007</v>
       </c>
       <c r="B42" t="s">
@@ -1183,13 +1199,40 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>240030</v>
       </c>
       <c r="B65" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <f t="shared" si="1"/>
+        <v>240031</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" s="6">
+        <v>19.97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <f t="shared" si="1"/>
+        <v>240032</v>
+      </c>
+      <c r="B67" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>